<commit_message>
Trabajando las fechas y extensiones en twig
</commit_message>
<xml_diff>
--- a/backup/cuenta_3940694600.xlsx
+++ b/backup/cuenta_3940694600.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\php-projects\dml2\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dml2\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="344">
   <si>
     <t>13051694-MOVISTAR -CB-7872717</t>
   </si>
@@ -1044,6 +1044,18 @@
   </si>
   <si>
     <t>260.34</t>
+  </si>
+  <si>
+    <t>13359401-MASTERCARD-RA-518114000072</t>
+  </si>
+  <si>
+    <t>0001621209</t>
+  </si>
+  <si>
+    <t>234.40  </t>
+  </si>
+  <si>
+    <t>3.40</t>
   </si>
 </sst>
 </file>
@@ -1366,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,29 +1393,29 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41718</v>
+        <v>41719</v>
       </c>
       <c r="B1" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-20'), 'mo_concepto' =&gt; '3940694600/0998453098', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008863007', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 2.00  , 'mo_saldo' =&gt; 237.80, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-20 21:10:46'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H4" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-21'), 'mo_concepto' =&gt; '13359401-MASTERCARD-RA-518114000072', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0001621209', 'mo_oficina' =&gt; 'SERVICIOS CENTRALES', 'mo_monto' =&gt; 234.40  , 'mo_saldo' =&gt; 3.40, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-21 9:42:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,26 +1423,22 @@
         <v>41718</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>329</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-20'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008214553', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 20.54  , 'mo_saldo' =&gt; 239.80, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-20 21:10:46'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1438,49 +1446,45 @@
         <v>41718</v>
       </c>
       <c r="B3" t="s">
-        <v>336</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>338</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>192</v>
+        <v>334</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-20'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008036516', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 40.00  , 'mo_saldo' =&gt; 260.34, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-20 21:10:46'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41717</v>
+        <v>41718</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>336</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>270</v>
+        <v>337</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>338</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>37</v>
+        <v>192</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>271</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1488,7 +1492,7 @@
         <v>41717</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1500,10 +1504,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1511,22 +1515,22 @@
         <v>41717</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1534,22 +1538,22 @@
         <v>41717</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1557,7 +1561,7 @@
         <v>41717</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1569,10 +1573,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1580,22 +1584,22 @@
         <v>41717</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>279</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1603,22 +1607,22 @@
         <v>41717</v>
       </c>
       <c r="B10" t="s">
-        <v>281</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1626,45 +1630,45 @@
         <v>41717</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>281</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>192</v>
+        <v>283</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41716</v>
+        <v>41717</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>288</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1678,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -1687,7 +1691,7 @@
         <v>32</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1695,45 +1699,45 @@
         <v>41716</v>
       </c>
       <c r="B14" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>293</v>
+        <v>32</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>33</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41715</v>
+        <v>41716</v>
       </c>
       <c r="B15" t="s">
-        <v>258</v>
+        <v>291</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>296</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,22 +1745,22 @@
         <v>41715</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>258</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>37</v>
+        <v>295</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1764,7 +1768,7 @@
         <v>41715</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1776,10 +1780,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1787,22 +1791,22 @@
         <v>41715</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>301</v>
+        <v>40</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1810,22 +1814,22 @@
         <v>41715</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>37</v>
+        <v>301</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1833,7 +1837,7 @@
         <v>41715</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1845,10 +1849,10 @@
         <v>2</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1856,22 +1860,22 @@
         <v>41715</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1879,22 +1883,22 @@
         <v>41715</v>
       </c>
       <c r="B22" t="s">
-        <v>309</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>175</v>
+        <v>307</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1902,22 +1906,22 @@
         <v>41715</v>
       </c>
       <c r="B23" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>314</v>
+        <v>175</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1925,22 +1929,22 @@
         <v>41715</v>
       </c>
       <c r="B24" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1948,7 +1952,7 @@
         <v>41715</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>316</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1960,10 +1964,10 @@
         <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1971,7 +1975,7 @@
         <v>41715</v>
       </c>
       <c r="B26" t="s">
-        <v>322</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1983,10 +1987,10 @@
         <v>10</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1994,114 +1998,114 @@
         <v>41715</v>
       </c>
       <c r="B27" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41712</v>
+        <v>41715</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>325</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>265</v>
+        <v>326</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>266</v>
+        <v>327</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>267</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41711</v>
+        <v>41712</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>32</v>
+        <v>266</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41709</v>
+        <v>41711</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>175</v>
+        <v>32</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41708</v>
+        <v>41709</v>
       </c>
       <c r="B31" t="s">
-        <v>258</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2109,22 +2113,22 @@
         <v>41708</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2132,22 +2136,22 @@
         <v>41708</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>59</v>
+        <v>263</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2155,22 +2159,22 @@
         <v>41708</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E34" t="s">
         <v>58</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2178,22 +2182,22 @@
         <v>41708</v>
       </c>
       <c r="B35" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E35" t="s">
         <v>58</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>254</v>
+        <v>62</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2201,68 +2205,68 @@
         <v>41708</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="E36" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>32</v>
+        <v>254</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41705</v>
+        <v>41708</v>
       </c>
       <c r="B37" t="s">
-        <v>243</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E37" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>243</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="E38" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>227</v>
+        <v>22</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,22 +2274,22 @@
         <v>41703</v>
       </c>
       <c r="B39" t="s">
-        <v>229</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2293,22 +2297,22 @@
         <v>41703</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>229</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2316,22 +2320,22 @@
         <v>41703</v>
       </c>
       <c r="B41" t="s">
-        <v>236</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E41" t="s">
-        <v>238</v>
+        <v>10</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2339,45 +2343,45 @@
         <v>41703</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>236</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>238</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>32</v>
+        <v>239</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B43" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E43" t="s">
         <v>140</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>211</v>
+        <v>32</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2385,22 +2389,22 @@
         <v>41698</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>209</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2408,68 +2412,68 @@
         <v>41698</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E45" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41697</v>
+        <v>41698</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>219</v>
+        <v>3</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41696</v>
+        <v>41697</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2477,7 +2481,7 @@
         <v>41696</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -2489,10 +2493,10 @@
         <v>2</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2500,68 +2504,68 @@
         <v>41696</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E49" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41690</v>
+        <v>41696</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="E50" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>197</v>
+        <v>108</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41689</v>
+        <v>41690</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E51" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2569,7 +2573,7 @@
         <v>41689</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -2581,10 +2585,10 @@
         <v>2</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2592,22 +2596,22 @@
         <v>41689</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E53" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2615,45 +2619,45 @@
         <v>41689</v>
       </c>
       <c r="B54" t="s">
-        <v>204</v>
+        <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E54" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41687</v>
+        <v>41689</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="E55" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2661,22 +2665,22 @@
         <v>41687</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E56" t="s">
         <v>2</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2684,7 +2688,7 @@
         <v>41687</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -2696,10 +2700,10 @@
         <v>2</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2707,22 +2711,22 @@
         <v>41687</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E58" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2730,22 +2734,22 @@
         <v>41687</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2753,45 +2757,45 @@
         <v>41687</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E60" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>41684</v>
+        <v>41687</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E61" t="s">
-        <v>191</v>
+        <v>18</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2799,45 +2803,45 @@
         <v>41684</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E62" t="s">
-        <v>31</v>
+        <v>191</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41682</v>
+        <v>41684</v>
       </c>
       <c r="B63" t="s">
-        <v>144</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="E63" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,22 +2849,22 @@
         <v>41682</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E64" t="s">
         <v>58</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2868,22 +2872,22 @@
         <v>41682</v>
       </c>
       <c r="B65" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E65" t="s">
         <v>58</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2891,45 +2895,45 @@
         <v>41682</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="C66" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E66" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41681</v>
+        <v>41682</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2937,22 +2941,22 @@
         <v>41681</v>
       </c>
       <c r="B68" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2966,16 +2970,16 @@
         <v>1</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E69" t="s">
         <v>10</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2983,45 +2987,45 @@
         <v>41681</v>
       </c>
       <c r="B70" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E70" t="s">
-        <v>169</v>
+        <v>10</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>41680</v>
+        <v>41681</v>
       </c>
       <c r="B71" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E71" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3029,45 +3033,45 @@
         <v>41680</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="E72" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B73" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="E73" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3075,22 +3079,22 @@
         <v>41677</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E74" t="s">
         <v>58</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3098,45 +3102,45 @@
         <v>41677</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E75" t="s">
         <v>58</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3144,22 +3148,22 @@
         <v>41676</v>
       </c>
       <c r="B77" t="s">
-        <v>123</v>
+        <v>13</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E77" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3167,22 +3171,22 @@
         <v>41676</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E78" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3196,16 +3200,16 @@
         <v>1</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E79" t="s">
         <v>18</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3213,68 +3217,68 @@
         <v>41676</v>
       </c>
       <c r="B80" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E80" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>41675</v>
+        <v>41676</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="C81" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E81" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>41674</v>
+        <v>41675</v>
       </c>
       <c r="B82" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>18</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3282,22 +3286,22 @@
         <v>41674</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="E83" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3305,7 +3309,7 @@
         <v>41674</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -3317,10 +3321,10 @@
         <v>2</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3328,45 +3332,45 @@
         <v>41674</v>
       </c>
       <c r="B85" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C85" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="E86" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3374,137 +3378,137 @@
         <v>41670</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E87" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>41663</v>
+        <v>41670</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>41662</v>
+        <v>41663</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>41661</v>
+        <v>41662</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E90" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>41656</v>
+        <v>41661</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E91" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>41655</v>
+        <v>41656</v>
       </c>
       <c r="B92" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E92" t="s">
         <v>2</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3512,22 +3516,22 @@
         <v>41655</v>
       </c>
       <c r="B93" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E93" t="s">
         <v>2</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3535,68 +3539,68 @@
         <v>41655</v>
       </c>
       <c r="B94" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E94" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>41654</v>
+        <v>41655</v>
       </c>
       <c r="B95" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E95" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>41653</v>
+        <v>41654</v>
       </c>
       <c r="B96" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E96" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3604,7 +3608,7 @@
         <v>41653</v>
       </c>
       <c r="B97" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
@@ -3616,10 +3620,10 @@
         <v>2</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3627,45 +3631,45 @@
         <v>41653</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E98" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>41652</v>
+        <v>41653</v>
       </c>
       <c r="B99" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C99" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E99" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3673,22 +3677,22 @@
         <v>41652</v>
       </c>
       <c r="B100" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E100" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -3696,22 +3700,22 @@
         <v>41652</v>
       </c>
       <c r="B101" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E101" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3719,22 +3723,22 @@
         <v>41652</v>
       </c>
       <c r="B102" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E102" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3742,7 +3746,7 @@
         <v>41652</v>
       </c>
       <c r="B103" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -3754,10 +3758,10 @@
         <v>2</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3765,22 +3769,22 @@
         <v>41652</v>
       </c>
       <c r="B104" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C104" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E104" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3788,45 +3792,45 @@
         <v>41652</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C105" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E105" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B106" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E106" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3834,7 +3838,7 @@
         <v>41649</v>
       </c>
       <c r="B107" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
@@ -3846,10 +3850,10 @@
         <v>2</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3857,22 +3861,22 @@
         <v>41649</v>
       </c>
       <c r="B108" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E108" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3880,22 +3884,22 @@
         <v>41649</v>
       </c>
       <c r="B109" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E109" t="s">
         <v>58</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3903,22 +3907,22 @@
         <v>41649</v>
       </c>
       <c r="B110" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E110" t="s">
         <v>58</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3926,45 +3930,45 @@
         <v>41649</v>
       </c>
       <c r="B111" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E111" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B112" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="C112" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E112" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3972,21 +3976,44 @@
         <v>41648</v>
       </c>
       <c r="B113" t="s">
+        <v>69</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E113" t="s">
+        <v>2</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B114" t="s">
         <v>16</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>17</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E114" t="s">
         <v>18</v>
       </c>
-      <c r="F113" s="3" t="s">
+      <c r="F114" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G113" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando ingreso por usuario logueado
</commit_message>
<xml_diff>
--- a/backup/cuenta_3940694600.xlsx
+++ b/backup/cuenta_3940694600.xlsx
@@ -2281,7 +2281,7 @@
   <dimension ref="A1:H220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,8 +2314,8 @@
         <v>71</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H49" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002663087', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 29.83  , 'mo_saldo' =&gt; 0.00, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-24 20:44:24'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H2" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002663087', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 29.83  , 'mo_saldo' =&gt; 0.00, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-25 12:4:44'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002662032', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 16.10  , 'mo_saldo' =&gt; 29.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-24 20:44:24'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002662032', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 16.10  , 'mo_saldo' =&gt; 29.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-25 12:4:44'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>